<commit_message>
Corrección error: exportación de tablas "Ninguno" e "Izquierda Extraparlamentaria"
</commit_message>
<xml_diff>
--- a/output/CEP-Datasets/V.2CEP-Idpart-Izquierda-Extraconcertacion-Edad.xlsx
+++ b/output/CEP-Datasets/V.2CEP-Idpart-Izquierda-Extraconcertacion-Edad.xlsx
@@ -426,37 +426,37 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.254468349961912</v>
+        <v>0.028692680627711</v>
       </c>
       <c r="C2">
-        <v>0.2420827885657363</v>
+        <v>0.03873025157783737</v>
       </c>
       <c r="D2">
-        <v>0.3202896541696007</v>
+        <v>0.01263319583351971</v>
       </c>
       <c r="E2">
-        <v>0.4227915798270814</v>
+        <v>0.0358191081401645</v>
       </c>
       <c r="F2">
-        <v>0.4035595204743503</v>
+        <v>0.05526694318194186</v>
       </c>
       <c r="G2">
-        <v>0.4247944345606114</v>
+        <v>0.05181147572192901</v>
       </c>
       <c r="H2">
-        <v>0.5294831662351244</v>
+        <v>0.04812787303689326</v>
       </c>
       <c r="I2">
-        <v>0.5905783715307758</v>
+        <v>0.03159878169708157</v>
       </c>
       <c r="J2">
-        <v>0.7079206503914106</v>
+        <v>0.01155715291314707</v>
       </c>
       <c r="K2">
-        <v>0.7961794101551293</v>
+        <v>0.01861302552872287</v>
       </c>
       <c r="L2">
-        <v>0.8187300229383669</v>
+        <v>0.038113883352762</v>
       </c>
     </row>
     <row r="3">
@@ -466,37 +466,37 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.254502188373156</v>
+        <v>0.0254213528407077</v>
       </c>
       <c r="C3">
-        <v>0.2779364278132506</v>
+        <v>0.02732587332997253</v>
       </c>
       <c r="D3">
-        <v>0.3623855023202564</v>
+        <v>0.0202914975688418</v>
       </c>
       <c r="E3">
-        <v>0.4104354844872833</v>
+        <v>0.0264414658497892</v>
       </c>
       <c r="F3">
-        <v>0.4191626279265866</v>
+        <v>0.0217403166827178</v>
       </c>
       <c r="G3">
-        <v>0.445998117986312</v>
+        <v>0.02464925514519373</v>
       </c>
       <c r="H3">
-        <v>0.5845284273630917</v>
+        <v>0.02643469413039877</v>
       </c>
       <c r="I3">
-        <v>0.6235466312672784</v>
+        <v>0.0223336180570061</v>
       </c>
       <c r="J3">
-        <v>0.7498210826897468</v>
+        <v>0.0078325302161393</v>
       </c>
       <c r="K3">
-        <v>0.8064057440926217</v>
+        <v>0.0159358812572107</v>
       </c>
       <c r="L3">
-        <v>0.798992828715176</v>
+        <v>0.0249390324576177</v>
       </c>
     </row>
     <row r="4">
@@ -506,37 +506,37 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.267382285184143</v>
+        <v>0.0215818661329497</v>
       </c>
       <c r="C4">
-        <v>0.2852911917959076</v>
+        <v>0.02007100159419284</v>
       </c>
       <c r="D4">
-        <v>0.3795995545671547</v>
+        <v>0.0166351930526708</v>
       </c>
       <c r="E4">
-        <v>0.422860807866481</v>
+        <v>0.02098971138387524</v>
       </c>
       <c r="F4">
-        <v>0.414498263414715</v>
+        <v>0.01854822079958457</v>
       </c>
       <c r="G4">
-        <v>0.447331122098401</v>
+        <v>0.02004964564012024</v>
       </c>
       <c r="H4">
-        <v>0.5721587957431926</v>
+        <v>0.02118492761448723</v>
       </c>
       <c r="I4">
-        <v>0.631070773183107</v>
+        <v>0.01391382112455054</v>
       </c>
       <c r="J4">
-        <v>0.7142630594484394</v>
+        <v>0.005884234056310167</v>
       </c>
       <c r="K4">
-        <v>0.789454659409048</v>
+        <v>0.00158334257103795</v>
       </c>
       <c r="L4">
-        <v>0.8242270310270881</v>
+        <v>0.02019421166472205</v>
       </c>
     </row>
     <row r="5">
@@ -546,34 +546,34 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.302050289868075</v>
+        <v>0.0188540837508389</v>
       </c>
       <c r="C5">
-        <v>0.281446907255482</v>
+        <v>0.01742281676510567</v>
       </c>
       <c r="E5">
-        <v>0.4469800044977697</v>
+        <v>0.008737176003543963</v>
       </c>
       <c r="F5">
-        <v>0.4249710207178524</v>
+        <v>0.01148957549789413</v>
       </c>
       <c r="G5">
-        <v>0.4778989520497093</v>
+        <v>0.01598894832380124</v>
       </c>
       <c r="H5">
-        <v>0.5802659554460526</v>
+        <v>0.0115275175684763</v>
       </c>
       <c r="I5">
-        <v>0.6329549859709903</v>
+        <v>0.0118959649768428</v>
       </c>
       <c r="J5">
-        <v>0.7078409540086043</v>
+        <v>0.002741759786351817</v>
       </c>
       <c r="K5">
-        <v>0.7693156079298668</v>
+        <v>0.00165935852028116</v>
       </c>
       <c r="L5">
-        <v>0.8066163513018569</v>
+        <v>0.01921779057578885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>